<commit_message>
Added to documents directory
Added a README.md,
Jim's Case 1: Building Envelope Analysis paper, and
created a PDF of Parcel Data Aggregator and Analysis Tool_v2
</commit_message>
<xml_diff>
--- a/documents/Pat_Envelope_V4.xlsx
+++ b/documents/Pat_Envelope_V4.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JRDFiles\Courses\2105_Summer_Law\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19740" windowHeight="16520"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingEnvelope" sheetId="1" r:id="rId1"/>
@@ -19,10 +14,13 @@
   <definedNames>
     <definedName name="INPUTS">BuildingEnvelope!$Q$3:$T$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="130407"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -267,23 +265,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -329,9 +331,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -702,7 +708,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="114">
@@ -754,14 +760,14 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -801,13 +807,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -820,9 +826,9 @@
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -835,7 +841,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -857,45 +863,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -912,6 +891,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -919,7 +925,7 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1131,7 +1137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1166,7 +1172,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1343,45 +1349,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="B1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="11" width="5.85546875" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" customWidth="1"/>
-    <col min="13" max="13" width="27.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="16" width="8.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="11" width="5.83203125" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" customWidth="1"/>
+    <col min="13" max="13" width="27.5" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="16" width="8.5" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" customWidth="1"/>
+    <col min="19" max="19" width="12.5" customWidth="1"/>
+    <col min="21" max="21" width="18.5" customWidth="1"/>
+    <col min="24" max="24" width="15.83203125" customWidth="1"/>
     <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:23" ht="16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1397,14 +1403,14 @@
       <c r="M1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="N1" s="94" t="s">
         <v>68</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:23" ht="17" thickBot="1">
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1427,7 +1433,7 @@
       <c r="P2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" ht="17" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="6"/>
       <c r="D3" s="11" t="s">
@@ -1446,7 +1452,7 @@
       <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="100">
+      <c r="N3" s="91">
         <f>HLOOKUP(N$1,INPUTS,3)</f>
         <v>0.48</v>
       </c>
@@ -1454,34 +1460,34 @@
       <c r="P3" s="14">
         <v>1</v>
       </c>
-      <c r="Q3" s="102" t="s">
+      <c r="Q3" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="103" t="s">
+      <c r="R3" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="103" t="s">
+      <c r="S3" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="T3" s="103" t="s">
+      <c r="T3" s="94" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23" ht="18.75" customHeight="1">
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="108" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
       <c r="J4" s="12"/>
       <c r="K4" s="11"/>
       <c r="L4" s="3">
@@ -1490,7 +1496,7 @@
       <c r="M4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="101">
+      <c r="N4" s="92">
         <f>HLOOKUP(N$1,INPUTS,4)</f>
         <v>1</v>
       </c>
@@ -1498,30 +1504,30 @@
       <c r="P4" s="14">
         <v>2</v>
       </c>
-      <c r="Q4" s="102" t="s">
+      <c r="Q4" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="R4" s="102">
+      <c r="R4" s="93">
         <v>40</v>
       </c>
-      <c r="S4" s="102">
+      <c r="S4" s="93">
         <v>55</v>
       </c>
-      <c r="T4" s="104">
+      <c r="T4" s="95">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:23" ht="17" thickBot="1">
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="91"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="109"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="93" t="s">
+      <c r="G5" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
       <c r="L5" s="3">
@@ -1535,21 +1541,21 @@
       <c r="P5" s="14">
         <v>3</v>
       </c>
-      <c r="Q5" s="102" t="s">
+      <c r="Q5" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="105">
+      <c r="R5" s="96">
         <v>0.6</v>
       </c>
-      <c r="S5" s="105">
+      <c r="S5" s="96">
         <v>0.6</v>
       </c>
-      <c r="T5" s="106">
+      <c r="T5" s="97">
         <f>((R16*R17)-(((R16*R19)*R17)+((R16*R20)*R17)+((R16-(R16*R19)-(R16*R20))*(R18*R17)*2)))/(R16*R17)</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23" ht="16">
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
       <c r="D6" s="21"/>
@@ -1566,7 +1572,7 @@
       <c r="M6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="112">
+      <c r="N6" s="103">
         <f>HLOOKUP(N$1,INPUTS,6)</f>
         <v>2</v>
       </c>
@@ -1574,24 +1580,24 @@
       <c r="P6" s="14">
         <v>4</v>
       </c>
-      <c r="Q6" s="102" t="s">
+      <c r="Q6" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="R6" s="102">
+      <c r="R6" s="93">
         <v>1.4</v>
       </c>
-      <c r="S6" s="102">
+      <c r="S6" s="93">
         <v>2.5</v>
       </c>
-      <c r="T6" s="102">
+      <c r="T6" s="93">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23" ht="16">
       <c r="B7" s="2"/>
       <c r="C7" s="6"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="105" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="11"/>
@@ -1621,24 +1627,24 @@
       <c r="P7" s="14">
         <v>5</v>
       </c>
-      <c r="Q7" s="107" t="s">
+      <c r="Q7" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="R7" s="108">
+      <c r="R7" s="99">
         <v>40</v>
       </c>
-      <c r="S7" s="108">
+      <c r="S7" s="99">
         <v>55</v>
       </c>
-      <c r="T7" s="109">
+      <c r="T7" s="100">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" ht="16">
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="87"/>
+      <c r="E8" s="105"/>
       <c r="F8" s="11"/>
       <c r="G8" s="29">
         <f>1/N6</f>
@@ -1664,21 +1670,21 @@
       <c r="P8" s="14">
         <v>6</v>
       </c>
-      <c r="Q8" s="110" t="s">
+      <c r="Q8" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="R8" s="111">
+      <c r="R8" s="102">
         <v>2</v>
       </c>
-      <c r="S8" s="111">
+      <c r="S8" s="102">
         <v>2</v>
       </c>
-      <c r="T8" s="111">
+      <c r="T8" s="102">
         <v>2</v>
       </c>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23" ht="16">
       <c r="B9" s="2"/>
       <c r="C9" s="6"/>
       <c r="D9" s="25"/>
@@ -1695,7 +1701,7 @@
       <c r="M9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="99">
+      <c r="N9" s="90">
         <f>HLOOKUP(N$1,INPUTS,7)</f>
         <v>0.25</v>
       </c>
@@ -1703,33 +1709,33 @@
       <c r="P9" s="14">
         <v>7</v>
       </c>
-      <c r="Q9" s="102" t="s">
+      <c r="Q9" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="R9" s="113">
+      <c r="R9" s="104">
         <v>3</v>
       </c>
-      <c r="S9" s="113">
+      <c r="S9" s="104">
         <v>4</v>
       </c>
-      <c r="T9" s="113">
+      <c r="T9" s="104">
         <v>0.25</v>
       </c>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" ht="16">
       <c r="B10" s="2"/>
       <c r="C10" s="6"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="105" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="94">
+      <c r="G10" s="112">
         <f>+G7*I7</f>
         <v>3000</v>
       </c>
-      <c r="H10" s="94"/>
+      <c r="H10" s="112"/>
       <c r="I10" s="11"/>
       <c r="J10" s="28"/>
       <c r="K10" s="11"/>
@@ -1748,18 +1754,18 @@
       </c>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" ht="17" thickBot="1">
       <c r="B11" s="2"/>
       <c r="C11" s="6"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="87"/>
+      <c r="E11" s="105"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="95">
+      <c r="G11" s="113">
         <f>+G8+I8</f>
         <v>0.57499999999999996</v>
       </c>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
       <c r="J11" s="28"/>
       <c r="K11" s="11"/>
       <c r="L11" s="3">
@@ -1775,12 +1781,12 @@
       <c r="P11" s="14">
         <v>9</v>
       </c>
-      <c r="Q11" s="97" t="s">
+      <c r="Q11" s="88" t="s">
         <v>63</v>
       </c>
       <c r="W11" s="2"/>
     </row>
-    <row r="12" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" ht="17" thickBot="1">
       <c r="B12" s="2"/>
       <c r="C12" s="6"/>
       <c r="D12" s="25"/>
@@ -1804,7 +1810,7 @@
       </c>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="2:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" ht="19.5" customHeight="1" thickBot="1">
       <c r="B13" s="2"/>
       <c r="C13" s="6"/>
       <c r="D13" s="37"/>
@@ -1816,7 +1822,7 @@
         <f>IF((N2*N3)/((1/N6)+(1/(1000/N9))*(N10/N11))&gt;(N2*N4),N2*N4,(N2*N3)/((1/N6)+(1/(1000/N9))*(N10/N11)))</f>
         <v>5217.3913043478269</v>
       </c>
-      <c r="H13" s="96"/>
+      <c r="H13" s="87"/>
       <c r="I13" s="39" t="s">
         <v>8</v>
       </c>
@@ -1835,7 +1841,7 @@
       <c r="P13" s="14"/>
       <c r="W13" s="2"/>
     </row>
-    <row r="14" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:23" ht="16">
       <c r="B14" s="2"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1860,7 +1866,7 @@
       <c r="P14" s="14"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:23" ht="16">
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1887,7 +1893,7 @@
       <c r="P15" s="14"/>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:23" ht="17" thickBot="1">
       <c r="B16" s="6"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -1912,7 +1918,7 @@
       <c r="Q16" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="R16" s="98">
+      <c r="R16" s="89">
         <v>125</v>
       </c>
       <c r="S16" s="77">
@@ -1923,7 +1929,7 @@
       </c>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:28" ht="16">
       <c r="B17" s="6"/>
       <c r="C17" s="45" t="s">
         <v>25</v>
@@ -1948,7 +1954,7 @@
       <c r="Q17" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="R17" s="98">
+      <c r="R17" s="89">
         <v>25</v>
       </c>
       <c r="S17" s="77">
@@ -1959,7 +1965,7 @@
       </c>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:28" ht="18">
       <c r="B18" s="6"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
@@ -2001,7 +2007,7 @@
       </c>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="2:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:28" ht="17" thickBot="1">
       <c r="B19" s="1"/>
       <c r="C19" s="25"/>
       <c r="D19" s="11" t="s">
@@ -2045,7 +2051,7 @@
       </c>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:28" ht="16">
       <c r="B20" s="1"/>
       <c r="C20" s="52"/>
       <c r="D20" s="53" t="s">
@@ -2086,7 +2092,7 @@
       </c>
       <c r="W20" s="2"/>
     </row>
-    <row r="21" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:28" ht="16">
       <c r="B21" s="6"/>
       <c r="C21" s="57" t="s">
         <v>31</v>
@@ -2110,7 +2116,7 @@
       <c r="P21" s="14"/>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:28" ht="18">
       <c r="B22" s="6"/>
       <c r="C22" s="25"/>
       <c r="D22" s="11" t="s">
@@ -2143,7 +2149,7 @@
       <c r="P22" s="14"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:28" ht="16">
       <c r="B23" s="1"/>
       <c r="C23" s="25"/>
       <c r="D23" s="11"/>
@@ -2169,7 +2175,7 @@
       <c r="W23" s="2"/>
       <c r="X23" s="62"/>
     </row>
-    <row r="24" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:28" ht="16">
       <c r="B24" s="1"/>
       <c r="C24" s="25"/>
       <c r="D24" s="11"/>
@@ -2193,7 +2199,7 @@
       <c r="W24" s="63"/>
       <c r="X24" s="62"/>
     </row>
-    <row r="25" spans="2:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:28" ht="17" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="25"/>
       <c r="D25" s="42" t="s">
@@ -2226,7 +2232,7 @@
       </c>
       <c r="W25" s="2"/>
     </row>
-    <row r="26" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:28" ht="16">
       <c r="B26" s="1"/>
       <c r="C26" s="25"/>
       <c r="D26" s="42"/>
@@ -2246,7 +2252,7 @@
       <c r="S26" s="14"/>
       <c r="AB26" s="2"/>
     </row>
-    <row r="27" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:28" ht="16">
       <c r="B27" s="1"/>
       <c r="C27" s="52"/>
       <c r="D27" s="53" t="s">
@@ -2270,7 +2276,7 @@
       <c r="S27" s="14"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:28" ht="16">
       <c r="B28" s="1"/>
       <c r="C28" s="57" t="s">
         <v>35</v>
@@ -2289,7 +2295,7 @@
       <c r="S28" s="14"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:28" ht="16">
       <c r="B29" s="6"/>
       <c r="C29" s="25"/>
       <c r="D29" s="11" t="s">
@@ -2313,7 +2319,7 @@
       <c r="S29" s="14"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:28" ht="16">
       <c r="B30" s="6"/>
       <c r="C30" s="25"/>
       <c r="D30" s="11" t="s">
@@ -2337,7 +2343,7 @@
       <c r="S30" s="14"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:28" ht="16">
       <c r="B31" s="6"/>
       <c r="C31" s="52"/>
       <c r="D31" s="53" t="s">
@@ -2360,7 +2366,7 @@
       <c r="S31" s="14"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="2:28" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:28" ht="17" thickBot="1">
       <c r="B32" s="6"/>
       <c r="C32" s="69" t="s">
         <v>36</v>
@@ -2383,20 +2389,20 @@
       <c r="S32" s="14"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:28">
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
       <c r="S33" s="14"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:28" ht="16">
       <c r="B34" s="6"/>
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
       <c r="S34" s="14"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:28" ht="16">
       <c r="B35" s="6"/>
       <c r="L35" s="43"/>
       <c r="M35" s="14"/>
@@ -2408,7 +2414,7 @@
       <c r="S35" s="14"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:28" ht="16">
       <c r="B36" s="6"/>
       <c r="L36" s="43"/>
       <c r="M36" s="14"/>
@@ -2420,7 +2426,7 @@
       <c r="S36" s="14"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" ht="16">
       <c r="B37" s="2"/>
       <c r="C37" s="6"/>
       <c r="D37" s="43"/>
@@ -2441,7 +2447,7 @@
       <c r="S37" s="14"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="2:28" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:28" ht="16">
       <c r="B38" s="2"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -2462,7 +2468,7 @@
       <c r="S38" s="14"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:28">
       <c r="B39" s="2"/>
       <c r="D39" s="43"/>
       <c r="E39" s="43"/>
@@ -2482,7 +2488,7 @@
       <c r="S39" s="14"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:28">
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
       <c r="F40" s="43"/>
@@ -2501,7 +2507,7 @@
       <c r="S40" s="14"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:28">
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="43"/>
@@ -2520,7 +2526,7 @@
       <c r="S41" s="14"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:28">
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
       <c r="F42" s="43"/>
@@ -2539,7 +2545,7 @@
       <c r="S42" s="14"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:28">
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -2558,7 +2564,7 @@
       <c r="S43" s="14"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:28">
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
       <c r="F44" s="43"/>
@@ -2577,7 +2583,7 @@
       <c r="S44" s="14"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:28">
       <c r="D45" s="43"/>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
@@ -2596,7 +2602,7 @@
       <c r="S45" s="14"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:28">
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
@@ -2615,7 +2621,7 @@
       <c r="S46" s="14"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:28">
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
@@ -2634,7 +2640,7 @@
       <c r="S47" s="14"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="2:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:28">
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
@@ -2653,7 +2659,7 @@
       <c r="S48" s="14"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="4:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:28">
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
@@ -2672,7 +2678,7 @@
       <c r="S49" s="14"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="4:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:28">
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
       <c r="F50" s="43"/>
@@ -2691,7 +2697,7 @@
       <c r="S50" s="14"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="4:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:28">
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2701,7 +2707,7 @@
       <c r="S51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="4:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:28">
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -2711,7 +2717,7 @@
       <c r="S52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="4:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:28">
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2721,7 +2727,7 @@
       <c r="S53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="4:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:28">
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -2731,7 +2737,7 @@
       <c r="S54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="4:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:28">
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -2741,42 +2747,49 @@
       <c r="S55" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="8">
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:I11"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:I11"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="B3:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12">
       <c r="B3" s="76" t="s">
         <v>51</v>
       </c>
@@ -2799,7 +2812,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12">
       <c r="B4" s="77" t="s">
         <v>40</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12">
       <c r="B5" s="76" t="s">
         <v>42</v>
       </c>
@@ -2857,7 +2870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12">
       <c r="B6" s="77" t="s">
         <v>43</v>
       </c>
@@ -2889,7 +2902,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12">
       <c r="B7" s="76" t="s">
         <v>44</v>
       </c>
@@ -2921,7 +2934,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12">
       <c r="B8" s="76" t="s">
         <v>45</v>
       </c>
@@ -2951,7 +2964,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12">
       <c r="B9" s="77" t="s">
         <v>46</v>
       </c>
@@ -2981,7 +2994,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12">
       <c r="B10" s="77" t="s">
         <v>41</v>
       </c>
@@ -2993,7 +3006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12">
       <c r="B11" s="77" t="s">
         <v>47</v>
       </c>
@@ -3006,19 +3019,31 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>